<commit_message>
Trying to do new tests for Address Book
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20055" windowHeight="7695"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="20055" windowHeight="10245"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>name0Z&lt;;O</t>
+    <t>WFoy3C</t>
   </si>
   <si>
-    <t>namez( ? b&gt;h</t>
+    <t>zxi2</t>
+  </si>
+  <si>
+    <t>OHMknjWBY</t>
+  </si>
+  <si>
+    <t>ilx8y0R j</t>
+  </si>
+  <si>
+    <t>tUwtYMyC</t>
   </si>
 </sst>
 </file>
@@ -354,20 +363,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>